<commit_message>
Add calibrated output voltage setting
* Python script serial utility for sending DIS, MWR, MRD commands to
  device.
* Three-coefficient polynomial calibration implemented in firmware for
  closer matching of output voltage (looks pretty darn good)! Makes up
  for the crappiness / non-linearity of the PWM pseudo-DAC driving a
  load without a buffer.
* Connecting the plumbing for setting output voltage via serial in the
  SCBS firmware.
* Clean up some commented code garbage that was lying around.
</commit_message>
<xml_diff>
--- a/excel/design_calcs.xlsx
+++ b/excel/design_calcs.xlsx
@@ -8,34 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\scbs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CCF56F-32F6-4790-BCF2-9372A690019C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C376EAF7-6C17-4C90-8F0D-F679510C4431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{B10D0899-44E0-483A-A53D-58AE10D06E7B}"/>
+    <workbookView xWindow="2004" yWindow="1248" windowWidth="19128" windowHeight="10920" xr2:uid="{B10D0899-44E0-483A-A53D-58AE10D06E7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Design Calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="Output Voltage Calibration" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="A_v_amp">Sheet1!$B$6</definedName>
-    <definedName name="A_v_csense">Sheet1!$B$28</definedName>
-    <definedName name="Blob_A">Sheet1!$B$29</definedName>
-    <definedName name="C_comp">Sheet1!$B$11</definedName>
-    <definedName name="C_filt">Sheet1!$B$16</definedName>
-    <definedName name="f_c_filt">Sheet1!$B$17</definedName>
-    <definedName name="I_shunt_max">Sheet1!$B$25</definedName>
-    <definedName name="R_b_pwm">Sheet1!$B$20</definedName>
-    <definedName name="R_comp">Sheet1!$B$10</definedName>
-    <definedName name="R_db">Sheet1!$B$32</definedName>
-    <definedName name="R_dt">Sheet1!$B$33</definedName>
-    <definedName name="R_fb">Sheet1!$B$5</definedName>
-    <definedName name="R_filt">Sheet1!$B$15</definedName>
-    <definedName name="R_ft">Sheet1!$B$7</definedName>
-    <definedName name="R_shunt">Sheet1!$B$24</definedName>
-    <definedName name="R_ub">Sheet1!$B$31</definedName>
-    <definedName name="R_ut">Sheet1!$B$30</definedName>
-    <definedName name="V_be_2n3904">Sheet1!$B$18</definedName>
-    <definedName name="V_sense_max">Sheet1!$B$27</definedName>
-    <definedName name="V_shunt_max">Sheet1!$B$26</definedName>
+    <definedName name="A_v_amp">'Design Calculations'!$B$6</definedName>
+    <definedName name="A_v_csense">'Design Calculations'!$B$28</definedName>
+    <definedName name="Blob_A">'Design Calculations'!$B$29</definedName>
+    <definedName name="C_comp">'Design Calculations'!$B$11</definedName>
+    <definedName name="C_filt">'Design Calculations'!$B$16</definedName>
+    <definedName name="COEFF_CONST">'Output Voltage Calibration'!$H$20</definedName>
+    <definedName name="COEFF_X">'Output Voltage Calibration'!$G$20</definedName>
+    <definedName name="COEFF_X2">'Output Voltage Calibration'!$F$20</definedName>
+    <definedName name="COEFF_X3">'Output Voltage Calibration'!$E$20</definedName>
+    <definedName name="f_c_filt">'Design Calculations'!$B$17</definedName>
+    <definedName name="I_shunt_max">'Design Calculations'!$B$25</definedName>
+    <definedName name="R_b_pwm">'Design Calculations'!$B$20</definedName>
+    <definedName name="R_comp">'Design Calculations'!$B$10</definedName>
+    <definedName name="R_db">'Design Calculations'!$B$32</definedName>
+    <definedName name="R_dt">'Design Calculations'!$B$33</definedName>
+    <definedName name="R_fb">'Design Calculations'!$B$5</definedName>
+    <definedName name="R_filt">'Design Calculations'!$B$15</definedName>
+    <definedName name="R_ft">'Design Calculations'!$B$7</definedName>
+    <definedName name="R_shunt">'Design Calculations'!$B$24</definedName>
+    <definedName name="R_ub">'Design Calculations'!$B$31</definedName>
+    <definedName name="R_ut">'Design Calculations'!$B$30</definedName>
+    <definedName name="V_be_2n3904">'Design Calculations'!$B$18</definedName>
+    <definedName name="V_sense_max">'Design Calculations'!$B$27</definedName>
+    <definedName name="V_shunt_max">'Design Calculations'!$B$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,8 +61,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Value</t>
   </si>
@@ -189,6 +216,33 @@
   </si>
   <si>
     <t>R_b_pwm</t>
+  </si>
+  <si>
+    <t>Set Voltage</t>
+  </si>
+  <si>
+    <t>Output Voltage</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Estimated Offset</t>
+  </si>
+  <si>
+    <t>Offset Polynomial</t>
+  </si>
+  <si>
+    <t>COEFF_X^3</t>
+  </si>
+  <si>
+    <t>COEFF_X^2</t>
+  </si>
+  <si>
+    <t>COEFF_X</t>
+  </si>
+  <si>
+    <t>COEFF_CONST</t>
   </si>
 </sst>
 </file>
@@ -257,6 +311,1232 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Output Voltage Calibration'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Offset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Output Voltage Calibration'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Output Voltage Calibration'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.7000000000000013E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.13500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.18599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.22900000000000009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.2629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.28799999999999981</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.30399999999999983</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.31000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.30600000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C1AC-4509-83B9-4FADC1915451}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1956124383"/>
+        <c:axId val="1592653167"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Output Voltage Calibration'!$A$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Set Voltage</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Output Voltage Calibration'!$A$2:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Output Voltage Calibration'!$A$2:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-C1AC-4509-83B9-4FADC1915451}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Output Voltage Calibration'!$B$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Output Voltage</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Output Voltage Calibration'!$A$2:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.5</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Output Voltage Calibration'!$B$2:$B$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>9.9000000000000005E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.42299999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.86499999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.3140000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.7709999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.2370000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.7120000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.1960000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.69</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.194</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-C1AC-4509-83B9-4FADC1915451}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1956124383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1592653167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1592653167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1956124383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>112395</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>17145</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F664157A-2D2D-2285-5B14-348AAA13C6E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,8 +1839,8 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -892,4 +2172,233 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74033C46-ECD0-49B0-A6CD-7C94E59BEC5C}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.734375" customWidth="1"/>
+    <col min="2" max="2" width="17.5234375" customWidth="1"/>
+    <col min="4" max="4" width="17.15625" customWidth="1"/>
+    <col min="5" max="5" width="12.15625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="C2">
+        <f>B2-A2</f>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E2">
+        <f>COEFF_X3*A2^3+COEFF_X2*A2^2+COEFF_X*A2+COEFF_CONST</f>
+        <v>7.9586013986014142E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+      <c r="B3">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C11" si="0">B3-A3</f>
+        <v>-7.7000000000000013E-2</v>
+      </c>
+      <c r="E3">
+        <f>COEFF_X3*A3^3+COEFF_X2*A3^2+COEFF_X*A3+COEFF_CONST</f>
+        <v>-4.233473193473189E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="E4">
+        <f>COEFF_X3*A4^3+COEFF_X2*A4^2+COEFF_X*A4+COEFF_CONST</f>
+        <v>-0.13313076923076925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>1.5</v>
+      </c>
+      <c r="B5">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-0.18599999999999994</v>
+      </c>
+      <c r="E5">
+        <f>COEFF_X3*A5^3+COEFF_X2*A5^2+COEFF_X*A5+COEFF_CONST</f>
+        <v>-0.19777062937062931</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1.7709999999999999</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-0.22900000000000009</v>
+      </c>
+      <c r="E6">
+        <f>COEFF_X3*A6^3+COEFF_X2*A6^2+COEFF_X*A6+COEFF_CONST</f>
+        <v>-0.24122284382284379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>2.5</v>
+      </c>
+      <c r="B7">
+        <v>2.2370000000000001</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-0.2629999999999999</v>
+      </c>
+      <c r="E7">
+        <f>COEFF_X3*A7^3+COEFF_X2*A7^2+COEFF_X*A7+COEFF_CONST</f>
+        <v>-0.26845594405594397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>2.7120000000000002</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-0.28799999999999981</v>
+      </c>
+      <c r="E8">
+        <f>COEFF_X3*A8^3+COEFF_X2*A8^2+COEFF_X*A8+COEFF_CONST</f>
+        <v>-0.28443846153846142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>3.5</v>
+      </c>
+      <c r="B9">
+        <v>3.1960000000000002</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-0.30399999999999983</v>
+      </c>
+      <c r="E9">
+        <f>COEFF_X3*A9^3+COEFF_X2*A9^2+COEFF_X*A9+COEFF_CONST</f>
+        <v>-0.29413892773892769</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>3.69</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-0.31000000000000005</v>
+      </c>
+      <c r="E10">
+        <f>COEFF_X3*A10^3+COEFF_X2*A10^2+COEFF_X*A10+COEFF_CONST</f>
+        <v>-0.30252587412587417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>4.5</v>
+      </c>
+      <c r="B11">
+        <v>4.194</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-0.30600000000000005</v>
+      </c>
+      <c r="E11">
+        <f>COEFF_X3*A11^3+COEFF_X2*A11^2+COEFF_X*A11+COEFF_CONST</f>
+        <v>-0.31456783216783235</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" cm="1">
+        <f t="array" ref="E20:H20">LINEST(C2:C11,A2:A11^{1,2,3})</f>
+        <v>-6.6247086247086633E-3</v>
+      </c>
+      <c r="F20">
+        <v>7.2186480186480412E-2</v>
+      </c>
+      <c r="G20">
+        <v>-0.27827855477855512</v>
+      </c>
+      <c r="H20">
+        <v>7.9586013986014142E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add CELLSIM 4S documentation
</commit_message>
<xml_diff>
--- a/excel/design_calcs.xlsx
+++ b/excel/design_calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\scbs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C376EAF7-6C17-4C90-8F0D-F679510C4431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6BA451-014E-480D-BB18-12CEAB8C8F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2004" yWindow="1248" windowWidth="19128" windowHeight="10920" xr2:uid="{B10D0899-44E0-483A-A53D-58AE10D06E7B}"/>
+    <workbookView xWindow="-30960" yWindow="2920" windowWidth="17280" windowHeight="9980" xr2:uid="{B10D0899-44E0-483A-A53D-58AE10D06E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Design Calculations" sheetId="1" r:id="rId1"/>
@@ -624,7 +624,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Output Voltage Calibration'!$B$1</c15:sqref>
@@ -653,7 +653,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Output Voltage Calibration'!$A$2:$A$11</c15:sqref>
@@ -698,7 +698,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Output Voltage Calibration'!$B$2:$B$11</c15:sqref>
@@ -742,7 +742,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-C1AC-4509-83B9-4FADC1915451}"/>
                   </c:ext>
@@ -1839,8 +1839,8 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2061,7 +2061,8 @@
         <v>9</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <f>1/(1/3.9+1/3.9+1/3.9+1/4.3)</f>
+        <v>0.99821428571428561</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
@@ -2084,7 +2085,7 @@
       </c>
       <c r="B26">
         <f>I_shunt_max*0.001*R_shunt</f>
-        <v>0.2</v>
+        <v>0.19964285714285712</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -2104,7 +2105,7 @@
       </c>
       <c r="B28">
         <f>V_sense_max/V_shunt_max</f>
-        <v>16.499999999999996</v>
+        <v>16.529516994633276</v>
       </c>
       <c r="C28" t="s">
         <v>19</v>
@@ -2116,7 +2117,7 @@
       </c>
       <c r="B29">
         <f>V_sense_max/(V_shunt_max+V_sense_max)</f>
-        <v>0.94285714285714284</v>
+        <v>0.94295336258801921</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -2127,7 +2128,7 @@
         <v>5</v>
       </c>
       <c r="B30">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -2139,7 +2140,7 @@
       </c>
       <c r="B31" s="1">
         <f>Blob_A/(1-Blob_A)*R_ut</f>
-        <v>8249.9999999999964</v>
+        <v>8430.0536672629732</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -2151,7 +2152,7 @@
       </c>
       <c r="B32" s="1">
         <f>R_ub</f>
-        <v>8249.9999999999964</v>
+        <v>8430.0536672629732</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -2163,7 +2164,7 @@
       </c>
       <c r="B33" s="1">
         <f>R_ut</f>
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -2217,7 +2218,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="E2">
-        <f>COEFF_X3*A2^3+COEFF_X2*A2^2+COEFF_X*A2+COEFF_CONST</f>
+        <f t="shared" ref="E2:E11" si="0">COEFF_X3*A2^3+COEFF_X2*A2^2+COEFF_X*A2+COEFF_CONST</f>
         <v>7.9586013986014142E-2</v>
       </c>
     </row>
@@ -2229,11 +2230,11 @@
         <v>0.42299999999999999</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="0">B3-A3</f>
+        <f t="shared" ref="C3:C11" si="1">B3-A3</f>
         <v>-7.7000000000000013E-2</v>
       </c>
       <c r="E3">
-        <f>COEFF_X3*A3^3+COEFF_X2*A3^2+COEFF_X*A3+COEFF_CONST</f>
+        <f t="shared" si="0"/>
         <v>-4.233473193473189E-2</v>
       </c>
     </row>
@@ -2245,11 +2246,11 @@
         <v>0.86499999999999999</v>
       </c>
       <c r="C4">
+        <f t="shared" si="1"/>
+        <v>-0.13500000000000001</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="0"/>
-        <v>-0.13500000000000001</v>
-      </c>
-      <c r="E4">
-        <f>COEFF_X3*A4^3+COEFF_X2*A4^2+COEFF_X*A4+COEFF_CONST</f>
         <v>-0.13313076923076925</v>
       </c>
     </row>
@@ -2261,11 +2262,11 @@
         <v>1.3140000000000001</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>-0.18599999999999994</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>-0.18599999999999994</v>
-      </c>
-      <c r="E5">
-        <f>COEFF_X3*A5^3+COEFF_X2*A5^2+COEFF_X*A5+COEFF_CONST</f>
         <v>-0.19777062937062931</v>
       </c>
     </row>
@@ -2277,11 +2278,11 @@
         <v>1.7709999999999999</v>
       </c>
       <c r="C6">
+        <f t="shared" si="1"/>
+        <v>-0.22900000000000009</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>-0.22900000000000009</v>
-      </c>
-      <c r="E6">
-        <f>COEFF_X3*A6^3+COEFF_X2*A6^2+COEFF_X*A6+COEFF_CONST</f>
         <v>-0.24122284382284379</v>
       </c>
     </row>
@@ -2293,11 +2294,11 @@
         <v>2.2370000000000001</v>
       </c>
       <c r="C7">
+        <f t="shared" si="1"/>
+        <v>-0.2629999999999999</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>-0.2629999999999999</v>
-      </c>
-      <c r="E7">
-        <f>COEFF_X3*A7^3+COEFF_X2*A7^2+COEFF_X*A7+COEFF_CONST</f>
         <v>-0.26845594405594397</v>
       </c>
     </row>
@@ -2309,11 +2310,11 @@
         <v>2.7120000000000002</v>
       </c>
       <c r="C8">
+        <f t="shared" si="1"/>
+        <v>-0.28799999999999981</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>-0.28799999999999981</v>
-      </c>
-      <c r="E8">
-        <f>COEFF_X3*A8^3+COEFF_X2*A8^2+COEFF_X*A8+COEFF_CONST</f>
         <v>-0.28443846153846142</v>
       </c>
     </row>
@@ -2325,11 +2326,11 @@
         <v>3.1960000000000002</v>
       </c>
       <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-0.30399999999999983</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>-0.30399999999999983</v>
-      </c>
-      <c r="E9">
-        <f>COEFF_X3*A9^3+COEFF_X2*A9^2+COEFF_X*A9+COEFF_CONST</f>
         <v>-0.29413892773892769</v>
       </c>
     </row>
@@ -2341,11 +2342,11 @@
         <v>3.69</v>
       </c>
       <c r="C10">
+        <f t="shared" si="1"/>
+        <v>-0.31000000000000005</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
-        <v>-0.31000000000000005</v>
-      </c>
-      <c r="E10">
-        <f>COEFF_X3*A10^3+COEFF_X2*A10^2+COEFF_X*A10+COEFF_CONST</f>
         <v>-0.30252587412587417</v>
       </c>
     </row>
@@ -2357,11 +2358,11 @@
         <v>4.194</v>
       </c>
       <c r="C11">
+        <f t="shared" si="1"/>
+        <v>-0.30600000000000005</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="0"/>
-        <v>-0.30600000000000005</v>
-      </c>
-      <c r="E11">
-        <f>COEFF_X3*A11^3+COEFF_X2*A11^2+COEFF_X*A11+COEFF_CONST</f>
         <v>-0.31456783216783235</v>
       </c>
     </row>

</xml_diff>